<commit_message>
Add photos; Update BOM to support 12V systems; Update README.
</commit_message>
<xml_diff>
--- a/Electronics/EN02OP-PWR-BOM.xlsx
+++ b/Electronics/EN02OP-PWR-BOM.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63666A5B-3533-4774-8A02-596827C543FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAD76F76-DFC3-4FEB-961C-C06C2DBF97D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM_5V_EN02OP" sheetId="1" r:id="rId1"/>
+    <sheet name="BOM_12V_EN02OP" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="151">
   <si>
     <t>Quantity</t>
   </si>
@@ -478,6 +479,100 @@
   </si>
   <si>
     <t>Resistance:12kΩ;Tolerance:±1%;Power:100mW;Temperature Coefficient:±100ppm/℃;SMD</t>
+  </si>
+  <si>
+    <t>220pF</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Capacitance:220pF;Tolerance:±10%;Rated Voltage:50V;Capacitance:Temperature Coefficient:X7R;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>10k</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="161"/>
+      </rPr>
+      <t>Ω</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>82pF</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Capacitance:82pF;Tolerance:±10%;Rated Voltage:50V;Capacitance:Temperature Coefficient:X7R;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>R22</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R29</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>7m</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="161"/>
+      </rPr>
+      <t>Ω</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>169k</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="161"/>
+      </rPr>
+      <t>Ω</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R18</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>150pF</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Capacitance:150pF;Tolerance:±10%;Rated Voltage:50V;Capacitance:Temperature Coefficient:X7R;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -507,12 +602,18 @@
       <charset val="161"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -527,8 +628,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -870,21 +972,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.25" customWidth="1"/>
-    <col min="2" max="2" width="9.625" customWidth="1"/>
-    <col min="3" max="3" width="23.5" customWidth="1"/>
-    <col min="4" max="4" width="39.875" customWidth="1"/>
+    <col min="1" max="1" width="4.265625" customWidth="1"/>
+    <col min="2" max="2" width="9.59765625" customWidth="1"/>
+    <col min="3" max="3" width="23.46484375" customWidth="1"/>
+    <col min="4" max="4" width="39.86328125" customWidth="1"/>
     <col min="5" max="6" width="20" customWidth="1"/>
     <col min="7" max="7" width="72" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -907,7 +1009,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -930,7 +1032,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -953,7 +1055,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -976,7 +1078,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -999,7 +1101,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -1022,7 +1124,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -1045,7 +1147,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -1068,7 +1170,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>32</v>
       </c>
@@ -1091,7 +1193,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>35</v>
       </c>
@@ -1114,7 +1216,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>40</v>
       </c>
@@ -1137,7 +1239,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>43</v>
       </c>
@@ -1157,7 +1259,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>45</v>
       </c>
@@ -1177,7 +1279,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>47</v>
       </c>
@@ -1194,7 +1296,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>50</v>
       </c>
@@ -1217,7 +1319,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>54</v>
       </c>
@@ -1240,7 +1342,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>57</v>
       </c>
@@ -1260,7 +1362,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>61</v>
       </c>
@@ -1283,7 +1385,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="14.65" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>64</v>
       </c>
@@ -1306,7 +1408,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>68</v>
       </c>
@@ -1329,7 +1431,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>71</v>
       </c>
@@ -1352,7 +1454,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>74</v>
       </c>
@@ -1375,7 +1477,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>77</v>
       </c>
@@ -1398,7 +1500,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>80</v>
       </c>
@@ -1421,7 +1523,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>82</v>
       </c>
@@ -1441,7 +1543,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>85</v>
       </c>
@@ -1464,7 +1566,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>87</v>
       </c>
@@ -1487,7 +1589,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>91</v>
       </c>
@@ -1510,7 +1612,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>94</v>
       </c>
@@ -1533,7 +1635,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>97</v>
       </c>
@@ -1556,7 +1658,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>100</v>
       </c>
@@ -1579,7 +1681,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" ht="14.65" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>104</v>
       </c>
@@ -1602,7 +1704,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
         <v>39</v>
       </c>
@@ -1613,4 +1715,800 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8609C17F-DE7C-4EA8-9378-3E67D54EAADB}">
+  <dimension ref="A1:G34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B9" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="4.265625" customWidth="1"/>
+    <col min="2" max="2" width="9.59765625" customWidth="1"/>
+    <col min="3" max="3" width="23.46484375" customWidth="1"/>
+    <col min="4" max="4" width="39.86328125" customWidth="1"/>
+    <col min="5" max="6" width="20" customWidth="1"/>
+    <col min="7" max="7" width="72" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" t="s">
+        <v>30</v>
+      </c>
+      <c r="G9" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" t="s">
+        <v>33</v>
+      </c>
+      <c r="G10" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" t="s">
+        <v>36</v>
+      </c>
+      <c r="F11" t="s">
+        <v>114</v>
+      </c>
+      <c r="G11" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D14" t="s">
+        <v>116</v>
+      </c>
+      <c r="E14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15" t="s">
+        <v>39</v>
+      </c>
+      <c r="F15" t="s">
+        <v>117</v>
+      </c>
+      <c r="G15" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>54</v>
+      </c>
+      <c r="B16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16" t="s">
+        <v>53</v>
+      </c>
+      <c r="E16" t="s">
+        <v>39</v>
+      </c>
+      <c r="F16" t="s">
+        <v>51</v>
+      </c>
+      <c r="G16" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" t="s">
+        <v>56</v>
+      </c>
+      <c r="D17" t="s">
+        <v>120</v>
+      </c>
+      <c r="E17" t="s">
+        <v>39</v>
+      </c>
+      <c r="F17" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>61</v>
+      </c>
+      <c r="B18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" t="s">
+        <v>59</v>
+      </c>
+      <c r="D18" t="s">
+        <v>60</v>
+      </c>
+      <c r="E18" t="s">
+        <v>58</v>
+      </c>
+      <c r="F18" t="s">
+        <v>58</v>
+      </c>
+      <c r="G18" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="14.65" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
+        <v>64</v>
+      </c>
+      <c r="B19" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" t="s">
+        <v>62</v>
+      </c>
+      <c r="D19" t="s">
+        <v>63</v>
+      </c>
+      <c r="E19" t="s">
+        <v>39</v>
+      </c>
+      <c r="F19" t="s">
+        <v>121</v>
+      </c>
+      <c r="G19" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>68</v>
+      </c>
+      <c r="B20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" t="s">
+        <v>66</v>
+      </c>
+      <c r="D20" t="s">
+        <v>67</v>
+      </c>
+      <c r="E20" t="s">
+        <v>65</v>
+      </c>
+      <c r="F20" t="s">
+        <v>65</v>
+      </c>
+      <c r="G20" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>71</v>
+      </c>
+      <c r="B21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" t="s">
+        <v>70</v>
+      </c>
+      <c r="D21" t="s">
+        <v>67</v>
+      </c>
+      <c r="E21" t="s">
+        <v>69</v>
+      </c>
+      <c r="F21" t="s">
+        <v>69</v>
+      </c>
+      <c r="G21" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>74</v>
+      </c>
+      <c r="B22" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" t="s">
+        <v>73</v>
+      </c>
+      <c r="D22" t="s">
+        <v>67</v>
+      </c>
+      <c r="E22" t="s">
+        <v>72</v>
+      </c>
+      <c r="F22" t="s">
+        <v>72</v>
+      </c>
+      <c r="G22" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>77</v>
+      </c>
+      <c r="B23" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" t="s">
+        <v>76</v>
+      </c>
+      <c r="D23" t="s">
+        <v>67</v>
+      </c>
+      <c r="E23" t="s">
+        <v>75</v>
+      </c>
+      <c r="F23" t="s">
+        <v>75</v>
+      </c>
+      <c r="G23" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" s="1" customFormat="1" ht="14.65" x14ac:dyDescent="0.45">
+      <c r="A24" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>82</v>
+      </c>
+      <c r="B25" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" t="s">
+        <v>146</v>
+      </c>
+      <c r="D25" t="s">
+        <v>67</v>
+      </c>
+      <c r="E25" t="s">
+        <v>41</v>
+      </c>
+      <c r="F25" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>85</v>
+      </c>
+      <c r="B26" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26" t="s">
+        <v>84</v>
+      </c>
+      <c r="D26" t="s">
+        <v>67</v>
+      </c>
+      <c r="E26" t="s">
+        <v>83</v>
+      </c>
+      <c r="F26" t="s">
+        <v>83</v>
+      </c>
+      <c r="G26" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>91</v>
+      </c>
+      <c r="B28" t="s">
+        <v>7</v>
+      </c>
+      <c r="C28" t="s">
+        <v>143</v>
+      </c>
+      <c r="D28" t="s">
+        <v>67</v>
+      </c>
+      <c r="E28" t="s">
+        <v>40</v>
+      </c>
+      <c r="F28" t="s">
+        <v>40</v>
+      </c>
+      <c r="G28" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="14.65" x14ac:dyDescent="0.45">
+      <c r="A29" t="s">
+        <v>94</v>
+      </c>
+      <c r="B29" t="s">
+        <v>11</v>
+      </c>
+      <c r="C29" t="s">
+        <v>89</v>
+      </c>
+      <c r="D29" t="s">
+        <v>90</v>
+      </c>
+      <c r="E29" t="s">
+        <v>144</v>
+      </c>
+      <c r="F29" t="s">
+        <v>88</v>
+      </c>
+      <c r="G29" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" s="1" customFormat="1" ht="14.65" x14ac:dyDescent="0.45">
+      <c r="A30" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>100</v>
+      </c>
+      <c r="B31" t="s">
+        <v>11</v>
+      </c>
+      <c r="C31" t="s">
+        <v>96</v>
+      </c>
+      <c r="D31" t="s">
+        <v>67</v>
+      </c>
+      <c r="E31" t="s">
+        <v>95</v>
+      </c>
+      <c r="F31" t="s">
+        <v>95</v>
+      </c>
+      <c r="G31" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>104</v>
+      </c>
+      <c r="B32" t="s">
+        <v>11</v>
+      </c>
+      <c r="C32" t="s">
+        <v>98</v>
+      </c>
+      <c r="D32" t="s">
+        <v>99</v>
+      </c>
+      <c r="E32" t="s">
+        <v>39</v>
+      </c>
+      <c r="F32" t="s">
+        <v>123</v>
+      </c>
+      <c r="G32" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="14.65" x14ac:dyDescent="0.45">
+      <c r="A33" t="s">
+        <v>141</v>
+      </c>
+      <c r="B33" t="s">
+        <v>11</v>
+      </c>
+      <c r="C33" t="s">
+        <v>102</v>
+      </c>
+      <c r="D33" t="s">
+        <v>103</v>
+      </c>
+      <c r="E33" t="s">
+        <v>101</v>
+      </c>
+      <c r="F33" t="s">
+        <v>101</v>
+      </c>
+      <c r="G33" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <printOptions gridLines="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>